<commit_message>
bugs have been fixed  on checkout
</commit_message>
<xml_diff>
--- a/public/admin/reports/sales_report_All.xlsx
+++ b/public/admin/reports/sales_report_All.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="60">
   <si>
     <t>Order ID</t>
   </si>
@@ -154,6 +154,33 @@
     <t>Chironji Seeds (2 x 500gm)</t>
   </si>
   <si>
+    <t>f4997297-362d-450a-b1d9-320725609ea5</t>
+  </si>
+  <si>
+    <t>12/30/2024</t>
+  </si>
+  <si>
+    <t>791c62fd-46bb-46e4-9d54-7239b14c263e</t>
+  </si>
+  <si>
+    <t>Fresh and Natural Black Seeds (2 x 1kg)</t>
+  </si>
+  <si>
+    <t>742fdec7-21fd-4e77-b46c-87fa033b9fd1</t>
+  </si>
+  <si>
+    <t>Chironji Seeds (5 x 250gm)</t>
+  </si>
+  <si>
+    <t>6b4532c9-bd83-460d-803a-410e4deddf68</t>
+  </si>
+  <si>
+    <t>2c219e31-f87a-4a04-9443-2feaa9f93d3b</t>
+  </si>
+  <si>
+    <t>Chironji Seeds (3 x 1kg)</t>
+  </si>
+  <si>
     <t>53d29848-bbe1-4354-9ef1-50a1cdb7ad7b</t>
   </si>
   <si>
@@ -163,7 +190,7 @@
     <t>12/31/2024</t>
   </si>
   <si>
-    <t>Grand Total: ₹36669.94</t>
+    <t>Grand Total: ₹53181.94</t>
   </si>
 </sst>
 </file>
@@ -540,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E35"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -946,21 +973,174 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>1710</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="D24">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>684</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26">
+        <v>3758</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>3758</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>3758</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29">
+        <v>5596</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <v>5596</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31">
+        <v>5596</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32">
+        <v>4764</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33">
         <v>2985.44</v>
       </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>50</v>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>